<commit_message>
created own file for setting headers of the xlsx file
</commit_message>
<xml_diff>
--- a/pakker-template.xlsx
+++ b/pakker-template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heeids\Documents\Ciber-prosjekter\ETA-Posten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6735174F-683C-4F44-BA77-1C78E260CBEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5500903-0289-470E-8589-C42802875FF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19155" yWindow="4275" windowWidth="17670" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13575" yWindow="5955" windowWidth="17670" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Forsendelser" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Fra</t>
   </si>
@@ -48,15 +48,25 @@
     <t>Sendingsdato</t>
   </si>
   <si>
-    <t>15.12.2020</t>
+    <t>0024</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>7075</t>
+  </si>
+  <si>
+    <t>4200</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -90,9 +100,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,15 +386,15 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3"/>
-    <col min="5" max="7" width="9.140625" style="4"/>
+    <col min="3" max="3" width="13" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="5" max="7" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -394,83 +404,84 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>5030</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1472</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4">
+        <v>44183</v>
+      </c>
+      <c r="D2" s="2">
         <v>3.4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>30</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>12</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>5030</v>
-      </c>
-      <c r="B3" s="1">
-        <v>7012</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4">
+        <v>44184</v>
+      </c>
+      <c r="D3" s="2">
         <v>4.2</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>12</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>12</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>5030</v>
-      </c>
-      <c r="B4" s="1">
-        <v>268</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
+        <v>44185</v>
+      </c>
+      <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
code refactoring and customized headers for output file
</commit_message>
<xml_diff>
--- a/pakker-template.xlsx
+++ b/pakker-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heeids\Documents\Ciber-prosjekter\ETA-Posten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5500903-0289-470E-8589-C42802875FF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471588B4-5B15-4193-8016-7D75C2502C75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13575" yWindow="5955" windowWidth="17670" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="6720" windowWidth="17670" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forsendelser" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Fra</t>
   </si>
   <si>
     <t>Til</t>
-  </si>
-  <si>
-    <t>Vekt</t>
-  </si>
-  <si>
-    <t>Høyde</t>
-  </si>
-  <si>
-    <t>Bredde</t>
-  </si>
-  <si>
-    <t>Lengde</t>
   </si>
   <si>
     <t>Sendingsdato</t>
@@ -66,7 +54,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -102,7 +90,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,7 +374,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,80 +393,57 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2" s="4">
         <v>44183</v>
       </c>
-      <c r="D2" s="2">
-        <v>3.4</v>
-      </c>
-      <c r="E2" s="3">
-        <v>30</v>
-      </c>
-      <c r="F2" s="3">
-        <v>12</v>
-      </c>
-      <c r="G2" s="3">
-        <v>15</v>
-      </c>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="4">
         <v>44184</v>
       </c>
-      <c r="D3" s="2">
-        <v>4.2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3">
-        <v>12</v>
-      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4">
         <v>44185</v>
       </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>